<commit_message>
upload image,xlsx to db
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -11,31 +11,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+  <si>
+    <t>PID</t>
+  </si>
+  <si>
+    <t>PRODUCT_NAME</t>
+  </si>
+  <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>WEIGHT</t>
+  </si>
+  <si>
+    <t>ALCOHOL</t>
+  </si>
+  <si>
+    <t>cabbage</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>beetroot</t>
+  </si>
+  <si>
+    <t>spinach</t>
+  </si>
+  <si>
+    <t>broccoli</t>
+  </si>
+  <si>
+    <t>papaya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -51,11 +76,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -79,6 +113,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="20.86"/>
+    <col customWidth="1" min="4" max="4" width="33.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -93,33 +131,114 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3">
         <v>2.0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
+        <v>22.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
         <v>3.0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>31.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
         <v>4.0</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>4.0</v>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>